<commit_message>
json parsing and screenshot taking
1. parse json info
2. take screenshot of the url and add screenshot name to Dataframe
3. add meaning of the pagesource product list
</commit_message>
<xml_diff>
--- a/data/Liberation_Price Tracker SKU list.xlsx
+++ b/data/Liberation_Price Tracker SKU list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kang.y.5\OneDrive - Procter and Gamble\Documents\GitHub\liberation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pgone-my.sharepoint.com/personal/kim_mj_1_pg_com/Documents/Documents/요청/Byeul nim/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{B9FC6692-016C-1B49-BDFF-437A3454B9F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C68D497B-239E-4F99-8752-2FA79E3A97F2}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D409811-5909-4868-A002-0999182B01C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{082D8A25-05B0-4134-80F4-C81249D6F8B7}"/>
+    <workbookView xWindow="20370" yWindow="-3300" windowWidth="29040" windowHeight="15840" xr2:uid="{082D8A25-05B0-4134-80F4-C81249D6F8B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Price Tracking Product List" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="262">
   <si>
     <t>No</t>
     <phoneticPr fontId="2"/>
@@ -208,6 +208,10 @@
   </si>
   <si>
     <t>4902430377072</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=18622015409</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Competitor-1</t>
@@ -657,6 +661,10 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6205110708</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">P&amp;G </t>
     </r>
@@ -1080,16 +1088,241 @@
     <t>2. Please refer 2nd/3rd sheet how to get necessary info from 1) Naver Price Checker site and 2) Coupang (Coupang as a seller, not 3rd party)</t>
   </si>
   <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6205110708</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nv_mid=10090557342</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nv_mid=17422432665</t>
-  </si>
-  <si>
-    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=18622015409</t>
+    <t>P&amp;G 다우니 고농축 섬유유연제 레몬그라스와 달콤한 라일락향 1L</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6205084952</t>
+  </si>
+  <si>
+    <t>P&amp;G 다우니 고농축 베리베리와바닐라크림 1L</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6205110388</t>
+  </si>
+  <si>
+    <t>P&amp;G 다우니 퍼퓸 섬유유연제 미스티크 1L</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6999016004</t>
+  </si>
+  <si>
+    <t>P&amp;G 다우니 스프링 가든 러브 1L</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=22470992398</t>
+  </si>
+  <si>
+    <t>P&amp;G 다우니 퍼퓸 고농축 섬유유연제 보타니스 코튼 퓨어 러브 1L</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=18625174654</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=17262800193</t>
+  </si>
+  <si>
+    <t>다우니 퍼퓸 실속팩 미스티크 리필 1.6L</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=20703609360</t>
+  </si>
+  <si>
+    <t>P&amp;G 다우니 엑스퍼트 실내건조 리필 1.6L</t>
+  </si>
+  <si>
+    <t>P&amp;G 다우니 초고농축 섬유유연제 레몬그라스 라일락향 2L</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6205084317</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=5825518465</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 상쾌한향 용기형 370ml</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6182316144</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 다우니향 용기형 370ml</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 은은한향 370ml</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=5825519252</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=10335014076</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 섬유탈취제 MEN 쿨아쿠아향 370ml</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 상쾌한향 실속형 900ml</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=5825518967</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 에어 맑은하늘바람 275g</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=23076875490</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=5825510700</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 상쾌한향 보충형 리필 320ml</t>
+  </si>
+  <si>
+    <t>한국P&amp;G 페브리즈 에어 섬유탈취제 다우니향 275g 1개</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6973866336</t>
+  </si>
+  <si>
+    <t>P&amp;G 페브리즈 섬유탈취제 대용량 다우니향 900ml</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/detail.nhn?nvMid=6746609696</t>
+  </si>
+  <si>
+    <t>페브리즈 화장실용 비치형 상쾌한 비누향 2입 1개</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/lite.nhn?nvMid=24030635784</t>
+  </si>
+  <si>
+    <t>페브리즈 차량용 방향제 2.2ml 맑은 하늘 바람</t>
+  </si>
+  <si>
+    <t>https://search.shopping.naver.com/detail/lite.nhn?nvMid=24075395989</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/324202666?itemId=1038077454</t>
+  </si>
+  <si>
+    <t>다우니 초고농축 섬유유연제 레몬그라스와 달콤한 라일락향 본품</t>
+  </si>
+  <si>
+    <t>다우니 초고농축 섬유유연제 핑크 베리베리와 바닐라크림향 본품</t>
+  </si>
+  <si>
+    <t>다우니 보타니스 섬유유연제 스프링가든러브 향</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/127467695?itemId=877623215</t>
+  </si>
+  <si>
+    <t>다우니 코튼 퓨어러브 본품</t>
+  </si>
+  <si>
+    <t>다우니 퍼퓸 초고농축 섬유유연제 미스티크 본품</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2237184136?itemId=3820245844</t>
+  </si>
+  <si>
+    <t>다우니 초고농축 섬유유연제 레몬그라스와 라일락향 본품</t>
+  </si>
+  <si>
+    <t>다우니 엑스퍼트 실내건조 섬유유연제 리필</t>
+  </si>
+  <si>
+    <t>다우니 초고농축 섬유유연제 레몬그라스와 달콤한 라일락 향 리필</t>
+  </si>
+  <si>
+    <t>JOBBER_PostS</t>
+  </si>
+  <si>
+    <t>JOBBER_Junimarket</t>
+  </si>
+  <si>
+    <t>다우니 섬유유연제 퍼퓸 미스티크 리필</t>
+  </si>
+  <si>
+    <t>JOBBER_World Shopping</t>
+  </si>
+  <si>
+    <t>페브리즈 섬유탈취제 상쾌한향 본품</t>
+  </si>
+  <si>
+    <t>페브리즈 섬유탈취제 다우니 에이프릴향 본품</t>
+  </si>
+  <si>
+    <t>페브리즈 섬유탈취제 은은한향 본품</t>
+  </si>
+  <si>
+    <t>페브리즈 포맨 쿨아쿠아향 본품</t>
+  </si>
+  <si>
+    <t>페브리즈 에어 실내탈취제 맑은 하늘바람 2p + 바닐라 라벤더의 포근함 2p</t>
+  </si>
+  <si>
+    <t>페브리즈 상쾌한향 섬유탈취제 리필</t>
+  </si>
+  <si>
+    <t>페브리즈 에어 맑은 하늘바람향 2개 + 다우니향 2개</t>
+  </si>
+  <si>
+    <t>페브리즈 화장실용 상쾌한 비누향 본품 6ml x 2p + 은은한 라벤더향 본품 6ml x 2p</t>
+  </si>
+  <si>
+    <t>페브리즈 차량용 맑은하늘바람</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/324202651?itemId=1038077401</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/1370801527?itemId=2403399112</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/159459703?itemId=176918955</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/206774214?itemId=610956818</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/304119666?itemId=957038309</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/5740084?itemId=6751262</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/1248271299?itemId=2247472071</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/264023657?itemId=827918246</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2992320?itemId=827918225</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/264023635?itemId=827918177</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/315183733?itemId=1001692867</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/165399844?itemId=474372068</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/2992229?itemId=421317</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/166986485?itemId=478216181</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/315183740?itemId=1001692898</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/264023639?itemId=827918181</t>
+  </si>
+  <si>
+    <t>https://www.coupang.com/vp/products/9565221?itemId=103784901</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1330,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1450,7 +1683,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1467,7 +1700,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1534,15 +1767,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1582,12 +1806,22 @@
     <xf numFmtId="0" fontId="16" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent1 2" xfId="3" xr:uid="{CD18BBF3-FE95-4D55-822D-0AA1A21D82CD}"/>
-    <cellStyle name="Hyperlink" xfId="18" builtinId="8"/>
     <cellStyle name="Input 2" xfId="2" xr:uid="{F20D85D8-ABDA-4BA0-9A6B-522473105DCE}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{E3027C87-3425-4354-A2E5-40D98544E226}"/>
     <cellStyle name="강조색1 2" xfId="11" xr:uid="{A934E348-EA5B-4334-AF0A-1E05D501C3AF}"/>
     <cellStyle name="나쁨 2" xfId="9" xr:uid="{C2AC1E40-D9C4-4553-9EC2-4A44D1F99467}"/>
@@ -1595,6 +1829,7 @@
     <cellStyle name="백분율 2 2 2" xfId="14" xr:uid="{2ABD8D88-0949-47C4-931B-E229CE8EC182}"/>
     <cellStyle name="쉼표 [0] 2 2 10 2" xfId="13" xr:uid="{985EC853-779B-4439-BD83-87878B8C29B7}"/>
     <cellStyle name="입력 2" xfId="10" xr:uid="{09712B67-15E2-4842-82AA-E3DCB3572D0B}"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
     <cellStyle name="표준 12" xfId="17" xr:uid="{A379F59E-3062-4AB9-BA52-A3E4F139F891}"/>
     <cellStyle name="표준 2" xfId="8" xr:uid="{4AF07777-0331-4824-9328-4B8C4FA9D6B8}"/>
     <cellStyle name="표준 2 2" xfId="12" xr:uid="{2449B9C0-4AAE-4931-880D-596972103349}"/>
@@ -1603,6 +1838,7 @@
     <cellStyle name="표준 3" xfId="15" xr:uid="{A157B020-D4AF-4EAE-B97C-42B65F5881CF}"/>
     <cellStyle name="표준 4" xfId="4" xr:uid="{99D950CB-BAA1-4230-A942-4E456B745BA6}"/>
     <cellStyle name="표준 5" xfId="6" xr:uid="{0A89C352-BF6C-489E-9EAF-1AE4462E684E}"/>
+    <cellStyle name="하이퍼링크" xfId="18" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3012,7 +3248,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3314,59 +3550,59 @@
       <pane xSplit="9" ySplit="11" topLeftCell="J12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" style="5" customWidth="1"/>
     <col min="6" max="6" width="9" style="5" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="7.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="5" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" style="5" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" style="5" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="5" customWidth="1"/>
     <col min="13" max="13" width="20.140625" style="5" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" style="5" customWidth="1"/>
     <col min="15" max="15" width="18.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="26.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="27" style="5" customWidth="1"/>
     <col min="19" max="19" width="29.42578125" style="5" customWidth="1"/>
     <col min="20" max="20" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" style="5" customWidth="1"/>
-    <col min="22" max="22" width="14.140625" style="5" customWidth="1"/>
-    <col min="23" max="23" width="15.140625" style="5" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" style="5" customWidth="1"/>
+    <col min="23" max="23" width="15.28515625" style="5" customWidth="1"/>
     <col min="24" max="27" width="23" style="5" customWidth="1"/>
     <col min="28" max="28" width="14" style="5" customWidth="1"/>
     <col min="29" max="29" width="30" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="30" style="5" customWidth="1"/>
-    <col min="31" max="31" width="23.7109375" style="5" customWidth="1"/>
+    <col min="31" max="31" width="23.5703125" style="5" customWidth="1"/>
     <col min="32" max="32" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.7109375" style="5" customWidth="1"/>
-    <col min="35" max="35" width="19.28515625" style="5" customWidth="1"/>
-    <col min="36" max="36" width="17.28515625" style="5" customWidth="1"/>
-    <col min="37" max="37" width="20.7109375" style="5" customWidth="1"/>
+    <col min="34" max="34" width="18.5703125" style="5" customWidth="1"/>
+    <col min="35" max="35" width="19.42578125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="17.42578125" style="5" customWidth="1"/>
+    <col min="37" max="37" width="20.5703125" style="5" customWidth="1"/>
     <col min="38" max="38" width="18.140625" style="5" customWidth="1"/>
     <col min="39" max="39" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="41" max="44" width="23" style="5" customWidth="1"/>
     <col min="45" max="45" width="14" style="5" customWidth="1"/>
     <col min="46" max="46" width="30" style="5" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="30" style="5" customWidth="1"/>
-    <col min="48" max="48" width="23.7109375" style="5" customWidth="1"/>
+    <col min="48" max="48" width="23.5703125" style="5" customWidth="1"/>
     <col min="49" max="49" width="20.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="18.7109375" style="5" customWidth="1"/>
-    <col min="52" max="52" width="19.28515625" style="5" customWidth="1"/>
-    <col min="53" max="53" width="17.28515625" style="5" customWidth="1"/>
-    <col min="54" max="54" width="20.7109375" style="5" customWidth="1"/>
+    <col min="51" max="51" width="18.5703125" style="5" customWidth="1"/>
+    <col min="52" max="52" width="19.42578125" style="5" customWidth="1"/>
+    <col min="53" max="53" width="17.42578125" style="5" customWidth="1"/>
+    <col min="54" max="54" width="20.5703125" style="5" customWidth="1"/>
     <col min="55" max="55" width="18.140625" style="5" customWidth="1"/>
     <col min="56" max="56" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
@@ -3375,47 +3611,47 @@
   <sheetData>
     <row r="1" spans="1:57" ht="21">
       <c r="A1" s="12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:57">
       <c r="A2" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:57">
       <c r="A3" s="5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:57">
       <c r="A4" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:57">
       <c r="A5" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:57">
       <c r="A6" s="5" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="V6" s="21" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="AO6" s="5" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:57">
@@ -3424,28 +3660,28 @@
     </row>
     <row r="8" spans="1:57" s="16" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B8" s="15"/>
       <c r="C8" s="15" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="15" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15"/>
       <c r="M8" s="15" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
@@ -3453,15 +3689,15 @@
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
       <c r="T8" s="15" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="U8" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="V8" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="W8" s="22"/>
+        <v>165</v>
+      </c>
+      <c r="V8" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="W8" s="37"/>
       <c r="X8" s="15"/>
       <c r="Y8" s="15"/>
       <c r="Z8" s="15"/>
@@ -3471,10 +3707,10 @@
       <c r="AD8" s="15"/>
       <c r="AE8" s="15"/>
       <c r="AF8" s="15" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AG8" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AH8" s="15"/>
       <c r="AI8" s="15"/>
@@ -3482,10 +3718,10 @@
       <c r="AK8" s="15"/>
       <c r="AL8" s="15"/>
       <c r="AM8" s="15" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AN8" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AO8" s="15"/>
       <c r="AP8" s="15"/>
@@ -3496,10 +3732,10 @@
       <c r="AU8" s="15"/>
       <c r="AV8" s="15"/>
       <c r="AW8" s="15" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="AX8" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="AY8" s="15"/>
       <c r="AZ8" s="15"/>
@@ -3507,169 +3743,169 @@
       <c r="BB8" s="15"/>
       <c r="BC8" s="15"/>
       <c r="BD8" s="15" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="BE8" s="15" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:57" ht="15.75">
       <c r="A9" s="14"/>
-      <c r="B9" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="30"/>
-      <c r="O9" s="30"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
-      <c r="S9" s="30"/>
-      <c r="T9" s="30"/>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="31"/>
-      <c r="X9" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="Y9" s="33"/>
-      <c r="Z9" s="33"/>
-      <c r="AA9" s="33"/>
-      <c r="AB9" s="33"/>
-      <c r="AC9" s="33"/>
-      <c r="AD9" s="33"/>
-      <c r="AE9" s="33"/>
-      <c r="AF9" s="33"/>
-      <c r="AG9" s="33"/>
-      <c r="AH9" s="33"/>
-      <c r="AI9" s="33"/>
-      <c r="AJ9" s="33"/>
-      <c r="AK9" s="33"/>
-      <c r="AL9" s="33"/>
-      <c r="AM9" s="33"/>
-      <c r="AN9" s="34"/>
-      <c r="AO9" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="AP9" s="36"/>
-      <c r="AQ9" s="36"/>
-      <c r="AR9" s="36"/>
-      <c r="AS9" s="36"/>
-      <c r="AT9" s="36"/>
-      <c r="AU9" s="36"/>
-      <c r="AV9" s="36"/>
-      <c r="AW9" s="36"/>
-      <c r="AX9" s="36"/>
-      <c r="AY9" s="36"/>
-      <c r="AZ9" s="36"/>
-      <c r="BA9" s="36"/>
-      <c r="BB9" s="36"/>
-      <c r="BC9" s="36"/>
-      <c r="BD9" s="36"/>
-      <c r="BE9" s="37"/>
+      <c r="B9" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="27"/>
+      <c r="P9" s="27"/>
+      <c r="Q9" s="27"/>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="27"/>
+      <c r="V9" s="27"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="30"/>
+      <c r="AC9" s="30"/>
+      <c r="AD9" s="30"/>
+      <c r="AE9" s="30"/>
+      <c r="AF9" s="30"/>
+      <c r="AG9" s="30"/>
+      <c r="AH9" s="30"/>
+      <c r="AI9" s="30"/>
+      <c r="AJ9" s="30"/>
+      <c r="AK9" s="30"/>
+      <c r="AL9" s="30"/>
+      <c r="AM9" s="30"/>
+      <c r="AN9" s="31"/>
+      <c r="AO9" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="AP9" s="33"/>
+      <c r="AQ9" s="33"/>
+      <c r="AR9" s="33"/>
+      <c r="AS9" s="33"/>
+      <c r="AT9" s="33"/>
+      <c r="AU9" s="33"/>
+      <c r="AV9" s="33"/>
+      <c r="AW9" s="33"/>
+      <c r="AX9" s="33"/>
+      <c r="AY9" s="33"/>
+      <c r="AZ9" s="33"/>
+      <c r="BA9" s="33"/>
+      <c r="BB9" s="33"/>
+      <c r="BC9" s="33"/>
+      <c r="BD9" s="33"/>
+      <c r="BE9" s="34"/>
     </row>
     <row r="10" spans="1:57">
       <c r="A10" s="4"/>
-      <c r="B10" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="25" t="s">
+      <c r="B10" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
-      <c r="U10" s="23"/>
-      <c r="V10" s="23"/>
-      <c r="W10" s="23"/>
-      <c r="X10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y10" s="24"/>
-      <c r="Z10" s="24"/>
-      <c r="AA10" s="24"/>
-      <c r="AB10" s="24"/>
-      <c r="AC10" s="25" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="P10" s="36"/>
+      <c r="Q10" s="36"/>
+      <c r="R10" s="36"/>
+      <c r="S10" s="36"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="36"/>
+      <c r="V10" s="36"/>
+      <c r="W10" s="36"/>
+      <c r="X10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AD10" s="25"/>
-      <c r="AE10" s="25"/>
-      <c r="AF10" s="25"/>
-      <c r="AG10" s="25"/>
-      <c r="AH10" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="AI10" s="23"/>
-      <c r="AJ10" s="23"/>
-      <c r="AK10" s="23"/>
-      <c r="AL10" s="23"/>
-      <c r="AM10" s="23"/>
-      <c r="AN10" s="23"/>
-      <c r="AO10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP10" s="24"/>
-      <c r="AQ10" s="24"/>
-      <c r="AR10" s="24"/>
-      <c r="AS10" s="24"/>
-      <c r="AT10" s="25" t="s">
+      <c r="Y10" s="35"/>
+      <c r="Z10" s="35"/>
+      <c r="AA10" s="35"/>
+      <c r="AB10" s="35"/>
+      <c r="AC10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AD10" s="22"/>
+      <c r="AE10" s="22"/>
+      <c r="AF10" s="22"/>
+      <c r="AG10" s="22"/>
+      <c r="AH10" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="AI10" s="36"/>
+      <c r="AJ10" s="36"/>
+      <c r="AK10" s="36"/>
+      <c r="AL10" s="36"/>
+      <c r="AM10" s="36"/>
+      <c r="AN10" s="36"/>
+      <c r="AO10" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AU10" s="25"/>
-      <c r="AV10" s="25"/>
-      <c r="AW10" s="25"/>
-      <c r="AX10" s="25"/>
-      <c r="AY10" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="AZ10" s="23"/>
-      <c r="BA10" s="23"/>
-      <c r="BB10" s="23"/>
-      <c r="BC10" s="23"/>
-      <c r="BD10" s="23"/>
-      <c r="BE10" s="23"/>
+      <c r="AP10" s="35"/>
+      <c r="AQ10" s="35"/>
+      <c r="AR10" s="35"/>
+      <c r="AS10" s="35"/>
+      <c r="AT10" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="AU10" s="22"/>
+      <c r="AV10" s="22"/>
+      <c r="AW10" s="22"/>
+      <c r="AX10" s="22"/>
+      <c r="AY10" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="AZ10" s="36"/>
+      <c r="BA10" s="36"/>
+      <c r="BB10" s="36"/>
+      <c r="BC10" s="36"/>
+      <c r="BD10" s="36"/>
+      <c r="BE10" s="36"/>
     </row>
     <row r="11" spans="1:57">
       <c r="A11" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>4</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>1</v>
@@ -3678,158 +3914,158 @@
         <v>2</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I11" s="17" t="s">
         <v>28</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="L11" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M11" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N11" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O11" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P11" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="Q11" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="S11" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="T11" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="U11" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="V11" s="17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W11" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X11" s="17" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="Y11" s="17" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="Z11" s="17" t="s">
         <v>4</v>
       </c>
       <c r="AA11" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AB11" s="17" t="s">
         <v>2</v>
       </c>
       <c r="AC11" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AD11" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AE11" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AF11" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AG11" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AH11" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AI11" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="AJ11" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AK11" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AL11" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AM11" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="AN11" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="AO11" s="17" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="AP11" s="17" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AQ11" s="17" t="s">
         <v>4</v>
       </c>
       <c r="AR11" s="17" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AS11" s="17" t="s">
         <v>2</v>
       </c>
       <c r="AT11" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AU11" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AV11" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AW11" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AX11" s="17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AY11" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AZ11" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="BA11" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="BB11" s="17" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="BC11" s="17" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="BD11" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="BE11" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:57" ht="16.5">
-      <c r="A12" s="5">
+      <c r="A12" s="38">
         <v>1</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -3837,10 +4073,10 @@
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>27</v>
@@ -3856,10 +4092,10 @@
         <v>18622015409</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>184</v>
+        <v>81</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>55</v>
       </c>
       <c r="M12" s="5">
         <v>1000</v>
@@ -3874,13 +4110,13 @@
         <v>2246825376</v>
       </c>
       <c r="Q12" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="R12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="S12" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="T12" s="5">
         <v>1050</v>
@@ -3888,12 +4124,9 @@
       <c r="U12" s="5">
         <v>3</v>
       </c>
-      <c r="AE12" s="1" t="s">
-        <v>183</v>
-      </c>
     </row>
     <row r="13" spans="1:57" ht="16.5">
-      <c r="A13" s="5">
+      <c r="A13" s="38">
         <v>2</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -3904,7 +4137,7 @@
         <v>17</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>27</v>
@@ -3920,10 +4153,10 @@
         <v>6205110708</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>181</v>
+        <v>83</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>82</v>
       </c>
       <c r="M13" s="5">
         <v>1000</v>
@@ -3938,13 +4171,13 @@
         <v>1038077450</v>
       </c>
       <c r="Q13" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="R13" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="S13" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="T13" s="5">
         <v>1050</v>
@@ -3952,12 +4185,9 @@
       <c r="U13" s="5">
         <v>3</v>
       </c>
-      <c r="AE13" s="1" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="14" spans="1:57">
-      <c r="A14" s="5">
+      <c r="A14" s="38">
         <v>3</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -3968,7 +4198,7 @@
         <v>18</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>27</v>
@@ -3980,9 +4210,45 @@
       <c r="I14" s="7">
         <v>3</v>
       </c>
+      <c r="J14" s="5">
+        <v>6205084952</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="M14" s="5">
+        <v>1000</v>
+      </c>
+      <c r="N14" s="5">
+        <v>1</v>
+      </c>
+      <c r="O14" s="5">
+        <v>324202666</v>
+      </c>
+      <c r="P14" s="5">
+        <v>1038077454</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R14" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="T14" s="5">
+        <v>1050</v>
+      </c>
+      <c r="U14" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:57">
-      <c r="A15" s="5">
+      <c r="A15" s="38">
         <v>4</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -3993,7 +4259,7 @@
         <v>19</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>27</v>
@@ -4005,9 +4271,45 @@
       <c r="I15" s="7">
         <v>4</v>
       </c>
+      <c r="J15" s="5">
+        <v>6205110388</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="M15" s="5">
+        <v>1000</v>
+      </c>
+      <c r="N15" s="5">
+        <v>1</v>
+      </c>
+      <c r="O15" s="5">
+        <v>324202651</v>
+      </c>
+      <c r="P15" s="5">
+        <v>1038077401</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="T15" s="5">
+        <v>1050</v>
+      </c>
+      <c r="U15" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:57">
-      <c r="A16" s="5">
+      <c r="A16" s="38">
         <v>5</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -4018,7 +4320,7 @@
         <v>20</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>27</v>
@@ -4030,9 +4332,45 @@
       <c r="I16" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="5">
+      <c r="J16" s="5">
+        <v>6999016004</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="M16" s="5">
+        <v>1000</v>
+      </c>
+      <c r="N16" s="5">
+        <v>1</v>
+      </c>
+      <c r="O16" s="5">
+        <v>2237184136</v>
+      </c>
+      <c r="P16" s="5">
+        <v>3820245844</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="T16" s="5">
+        <v>1050</v>
+      </c>
+      <c r="U16" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
+      <c r="A17" s="38">
         <v>6</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -4043,7 +4381,7 @@
         <v>21</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>27</v>
@@ -4055,9 +4393,45 @@
       <c r="I17" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="5">
+      <c r="J17" s="5">
+        <v>22470992398</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="M17" s="5">
+        <v>1000</v>
+      </c>
+      <c r="N17" s="5">
+        <v>1</v>
+      </c>
+      <c r="O17" s="5">
+        <v>1370801527</v>
+      </c>
+      <c r="P17" s="5">
+        <v>2403399112</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R17" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="T17" s="5">
+        <v>1050</v>
+      </c>
+      <c r="U17" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21">
+      <c r="A18" s="38">
         <v>7</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -4068,7 +4442,7 @@
         <v>22</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>27</v>
@@ -4080,9 +4454,45 @@
       <c r="I18" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="5">
+      <c r="J18" s="5">
+        <v>18625174654</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M18" s="5">
+        <v>1000</v>
+      </c>
+      <c r="N18" s="5">
+        <v>1</v>
+      </c>
+      <c r="O18" s="5">
+        <v>127467695</v>
+      </c>
+      <c r="P18" s="5">
+        <v>877623215</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="T18" s="5">
+        <v>1050</v>
+      </c>
+      <c r="U18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21">
+      <c r="A19" s="38">
         <v>8</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -4093,7 +4503,7 @@
         <v>23</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>27</v>
@@ -4105,9 +4515,30 @@
       <c r="I19" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="5">
+      <c r="O19" s="5">
+        <v>159459703</v>
+      </c>
+      <c r="P19" s="5">
+        <v>176918955</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="T19" s="5">
+        <v>1600</v>
+      </c>
+      <c r="U19" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21">
+      <c r="A20" s="38">
         <v>9</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -4118,7 +4549,7 @@
         <v>24</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>27</v>
@@ -4130,9 +4561,45 @@
       <c r="I20" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="5">
+      <c r="J20" s="5">
+        <v>20703609360</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="M20" s="5">
+        <v>1600</v>
+      </c>
+      <c r="N20" s="5">
+        <v>1</v>
+      </c>
+      <c r="O20" s="5">
+        <v>206774214</v>
+      </c>
+      <c r="P20" s="5">
+        <v>610956818</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="T20" s="5">
+        <v>1600</v>
+      </c>
+      <c r="U20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21">
+      <c r="A21" s="38">
         <v>10</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -4143,7 +4610,7 @@
         <v>25</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F21" s="7" t="s">
         <v>27</v>
@@ -4155,9 +4622,45 @@
       <c r="I21" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="5">
+      <c r="J21" s="5">
+        <v>17262800193</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="M21" s="5">
+        <v>1600</v>
+      </c>
+      <c r="N21" s="5">
+        <v>1</v>
+      </c>
+      <c r="O21" s="5">
+        <v>304119666</v>
+      </c>
+      <c r="P21" s="5">
+        <v>957038309</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="T21" s="5">
+        <v>1600</v>
+      </c>
+      <c r="U21" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21">
+      <c r="A22" s="38">
         <v>11</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -4168,7 +4671,7 @@
         <v>26</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F22" s="7" t="s">
         <v>27</v>
@@ -4180,9 +4683,45 @@
       <c r="I22" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="5">
+      <c r="J22" s="5">
+        <v>6205084317</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M22" s="5">
+        <v>2000</v>
+      </c>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+      <c r="O22" s="5">
+        <v>5740084</v>
+      </c>
+      <c r="P22" s="5">
+        <v>6751262</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="T22" s="5">
+        <v>2000</v>
+      </c>
+      <c r="U22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="38">
         <v>12</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -4193,10 +4732,10 @@
         <v>44</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G23" s="7" t="s">
         <v>43</v>
@@ -4207,9 +4746,45 @@
       <c r="I23" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="5">
+      <c r="J23" s="5">
+        <v>5825518465</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="M23" s="5">
+        <v>370</v>
+      </c>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
+      <c r="O23" s="5">
+        <v>1248271299</v>
+      </c>
+      <c r="P23" s="5">
+        <v>2247472071</v>
+      </c>
+      <c r="Q23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R23" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="T23" s="5">
+        <v>360</v>
+      </c>
+      <c r="U23" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21">
+      <c r="A24" s="38">
         <v>13</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -4220,10 +4795,10 @@
         <v>45</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G24" s="7" t="s">
         <v>43</v>
@@ -4234,9 +4809,45 @@
       <c r="I24" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="5">
+      <c r="J24" s="5">
+        <v>6182316144</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="M24" s="5">
+        <v>370</v>
+      </c>
+      <c r="N24" s="5">
+        <v>1</v>
+      </c>
+      <c r="O24" s="5">
+        <v>264023657</v>
+      </c>
+      <c r="P24" s="5">
+        <v>827918246</v>
+      </c>
+      <c r="Q24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T24" s="5">
+        <v>360</v>
+      </c>
+      <c r="U24" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21">
+      <c r="A25" s="38">
         <v>14</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -4247,10 +4858,10 @@
         <v>46</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G25" s="7" t="s">
         <v>43</v>
@@ -4261,9 +4872,45 @@
       <c r="I25" s="7">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="5">
+      <c r="J25" s="5">
+        <v>5825519252</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="M25" s="5">
+        <v>370</v>
+      </c>
+      <c r="N25" s="5">
+        <v>1</v>
+      </c>
+      <c r="O25" s="5">
+        <v>2992320</v>
+      </c>
+      <c r="P25" s="5">
+        <v>827918225</v>
+      </c>
+      <c r="Q25" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="T25" s="5">
+        <v>360</v>
+      </c>
+      <c r="U25" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21">
+      <c r="A26" s="38">
         <v>15</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -4274,10 +4921,10 @@
         <v>47</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>43</v>
@@ -4288,9 +4935,45 @@
       <c r="I26" s="7">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="5">
+      <c r="J26" s="5">
+        <v>10335014076</v>
+      </c>
+      <c r="K26" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="M26" s="5">
+        <v>370</v>
+      </c>
+      <c r="N26" s="5">
+        <v>1</v>
+      </c>
+      <c r="O26" s="5">
+        <v>264023635</v>
+      </c>
+      <c r="P26" s="5">
+        <v>827918177</v>
+      </c>
+      <c r="Q26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R26" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="T26" s="5">
+        <v>360</v>
+      </c>
+      <c r="U26" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21">
+      <c r="A27" s="38">
         <v>16</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -4301,10 +4984,10 @@
         <v>48</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>43</v>
@@ -4315,9 +4998,45 @@
       <c r="I27" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:9">
-      <c r="A28" s="5">
+      <c r="J27" s="5">
+        <v>5825518967</v>
+      </c>
+      <c r="K27" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="M27" s="5">
+        <v>900</v>
+      </c>
+      <c r="N27" s="5">
+        <v>1</v>
+      </c>
+      <c r="O27" s="5">
+        <v>315183733</v>
+      </c>
+      <c r="P27" s="5">
+        <v>1001692867</v>
+      </c>
+      <c r="Q27" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R27" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="T27" s="5">
+        <v>880</v>
+      </c>
+      <c r="U27" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" s="38">
         <v>17</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -4328,10 +5047,10 @@
         <v>49</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>43</v>
@@ -4342,9 +5061,45 @@
       <c r="I28" s="7">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="5">
+      <c r="J28" s="5">
+        <v>23076875490</v>
+      </c>
+      <c r="K28" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="M28" s="5">
+        <v>275</v>
+      </c>
+      <c r="N28" s="5">
+        <v>1</v>
+      </c>
+      <c r="O28" s="5">
+        <v>165399844</v>
+      </c>
+      <c r="P28" s="5">
+        <v>474372068</v>
+      </c>
+      <c r="Q28" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R28" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="T28" s="5">
+        <v>275</v>
+      </c>
+      <c r="U28" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="38">
         <v>18</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -4355,10 +5110,10 @@
         <v>50</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>43</v>
@@ -4369,9 +5124,45 @@
       <c r="I29" s="7">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:9">
-      <c r="A30" s="5">
+      <c r="J29" s="5">
+        <v>5825510700</v>
+      </c>
+      <c r="K29" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="M29" s="5">
+        <v>320</v>
+      </c>
+      <c r="N29" s="5">
+        <v>1</v>
+      </c>
+      <c r="O29" s="5">
+        <v>2992229</v>
+      </c>
+      <c r="P29" s="5">
+        <v>421317</v>
+      </c>
+      <c r="Q29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R29" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="T29" s="5">
+        <v>320</v>
+      </c>
+      <c r="U29" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
+      <c r="A30" s="38">
         <v>19</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -4382,10 +5173,10 @@
         <v>51</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G30" s="7" t="s">
         <v>43</v>
@@ -4396,9 +5187,45 @@
       <c r="I30" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="5">
+      <c r="J30" s="5">
+        <v>6973866336</v>
+      </c>
+      <c r="K30" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M30" s="5">
+        <v>275</v>
+      </c>
+      <c r="N30" s="5">
+        <v>1</v>
+      </c>
+      <c r="O30" s="5">
+        <v>166986485</v>
+      </c>
+      <c r="P30" s="5">
+        <v>478216181</v>
+      </c>
+      <c r="Q30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R30" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="T30" s="5">
+        <v>275</v>
+      </c>
+      <c r="U30" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21">
+      <c r="A31" s="38">
         <v>20</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -4409,10 +5236,10 @@
         <v>52</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G31" s="7" t="s">
         <v>43</v>
@@ -4423,9 +5250,45 @@
       <c r="I31" s="7">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="5">
+      <c r="J31" s="5">
+        <v>6746609696</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="M31" s="5">
+        <v>900</v>
+      </c>
+      <c r="N31" s="5">
+        <v>1</v>
+      </c>
+      <c r="O31" s="5">
+        <v>315183740</v>
+      </c>
+      <c r="P31" s="5">
+        <v>1001692898</v>
+      </c>
+      <c r="Q31" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R31" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="T31" s="5">
+        <v>880</v>
+      </c>
+      <c r="U31" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" s="38">
         <v>21</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -4436,10 +5299,10 @@
         <v>53</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G32" s="7" t="s">
         <v>43</v>
@@ -4450,9 +5313,45 @@
       <c r="I32" s="7">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="5">
+      <c r="J32" s="5">
+        <v>24030635784</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="M32" s="5">
+        <v>6</v>
+      </c>
+      <c r="N32" s="5">
+        <v>2</v>
+      </c>
+      <c r="O32" s="5">
+        <v>264023639</v>
+      </c>
+      <c r="P32" s="5">
+        <v>827918181</v>
+      </c>
+      <c r="Q32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R32" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="T32" s="5">
+        <v>6</v>
+      </c>
+      <c r="U32" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21">
+      <c r="A33" s="38">
         <v>22</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -4463,10 +5362,10 @@
         <v>54</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="G33" s="7" t="s">
         <v>43</v>
@@ -4477,407 +5376,443 @@
       <c r="I33" s="7">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="1:9">
+      <c r="J33" s="5">
+        <v>24075395989</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="M33" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N33" s="5">
+        <v>1</v>
+      </c>
+      <c r="O33" s="5">
+        <v>9565221</v>
+      </c>
+      <c r="P33" s="5">
+        <v>103784901</v>
+      </c>
+      <c r="Q33" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R33" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="T33" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U33" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" s="5">
         <v>23</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:21">
       <c r="A35" s="5">
         <v>24</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H35" s="7"/>
       <c r="I35" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:21">
       <c r="A36" s="5">
         <v>25</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H36" s="7"/>
       <c r="I36" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:21">
       <c r="A37" s="5">
         <v>26</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H37" s="7"/>
       <c r="I37" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:21">
       <c r="A38" s="5">
         <v>27</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:21">
       <c r="A39" s="5">
         <v>28</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:21">
       <c r="A40" s="5">
         <v>29</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H40" s="7"/>
       <c r="I40" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:21">
       <c r="A41" s="5">
         <v>30</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H41" s="7"/>
       <c r="I41" s="10">
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:21">
       <c r="A42" s="5">
         <v>31</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H42" s="7"/>
       <c r="I42" s="10">
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:21">
       <c r="A43" s="5">
         <v>32</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H43" s="7"/>
       <c r="I43" s="10">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:21">
       <c r="A44" s="5">
         <v>33</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H44" s="7"/>
       <c r="I44" s="10">
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:21">
       <c r="A45" s="5">
         <v>34</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H45" s="7"/>
       <c r="I45" s="10">
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:21">
       <c r="A46" s="5">
         <v>35</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H46" s="7"/>
       <c r="I46" s="10">
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:21">
       <c r="A47" s="5">
         <v>36</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H47" s="7"/>
       <c r="I47" s="10">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:21">
       <c r="A48" s="5">
         <v>37</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C48" s="10"/>
       <c r="D48" s="11" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H48" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I48" s="10">
         <v>1</v>
@@ -4888,23 +5823,23 @@
         <v>38</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C49" s="10"/>
       <c r="D49" s="11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I49" s="10">
         <v>2</v>
@@ -4915,23 +5850,23 @@
         <v>39</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="11" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G50" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I50" s="10">
         <v>3</v>
@@ -4942,23 +5877,23 @@
         <v>40</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="11" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G51" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I51" s="10">
         <v>4</v>
@@ -4969,23 +5904,23 @@
         <v>41</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C52" s="10"/>
       <c r="D52" s="11" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I52" s="10">
         <v>5</v>
@@ -4996,23 +5931,23 @@
         <v>42</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C53" s="10"/>
       <c r="D53" s="11" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I53" s="10">
         <v>6</v>
@@ -5023,23 +5958,23 @@
         <v>43</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C54" s="10"/>
       <c r="D54" s="11" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I54" s="10">
         <v>7</v>
@@ -5050,23 +5985,23 @@
         <v>44</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="11" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H55" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I55" s="10">
         <v>8</v>
@@ -5077,23 +6012,23 @@
         <v>45</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H56" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I56" s="10">
         <v>9</v>
@@ -5104,23 +6039,23 @@
         <v>46</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C57" s="10"/>
       <c r="D57" s="11" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H57" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I57" s="10">
         <v>10</v>
@@ -5131,23 +6066,23 @@
         <v>47</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C58" s="10"/>
       <c r="D58" s="11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H58" s="10" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I58" s="10">
         <v>11</v>
@@ -5320,6 +6255,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="O10:W10"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="AC10:AG10"/>
+    <mergeCell ref="AH10:AN10"/>
     <mergeCell ref="J10:N10"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B9:W9"/>
@@ -5328,11 +6268,6 @@
     <mergeCell ref="AO10:AS10"/>
     <mergeCell ref="AT10:AX10"/>
     <mergeCell ref="AY10:BE10"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="O10:W10"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="AC10:AG10"/>
-    <mergeCell ref="AH10:AN10"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -5340,11 +6275,48 @@
     <hyperlink ref="S13" r:id="rId2" xr:uid="{A7CAC174-3116-4EC3-AAF9-FBACA70DC46F}"/>
     <hyperlink ref="S12" r:id="rId3" xr:uid="{D370E371-22DA-4E1F-8346-20D041CE7652}"/>
     <hyperlink ref="L13" r:id="rId4" xr:uid="{8F2C1114-78B9-478D-B679-B541051B28B6}"/>
-    <hyperlink ref="AE13" r:id="rId5" xr:uid="{B845A19C-979D-4780-B34F-2D233CD0C141}"/>
-    <hyperlink ref="AE12" r:id="rId6" xr:uid="{FA66ED17-514E-41A3-BC17-506B5964A2B2}"/>
+    <hyperlink ref="L14" r:id="rId5" xr:uid="{0E3B742B-F12B-44CC-8914-38B7DE7C5290}"/>
+    <hyperlink ref="L15" r:id="rId6" xr:uid="{02D6E6EE-9E4C-4B42-80DF-B1EF4349A5D8}"/>
+    <hyperlink ref="L16" r:id="rId7" xr:uid="{6153E673-224E-48B8-927A-3D332BC7BECC}"/>
+    <hyperlink ref="L17" r:id="rId8" xr:uid="{92391632-4E84-4F1C-8D58-BBBFEE55BBCC}"/>
+    <hyperlink ref="L18" r:id="rId9" xr:uid="{C8DDECF5-CDB3-4049-B413-79B764839E19}"/>
+    <hyperlink ref="L21" r:id="rId10" xr:uid="{831A9323-EC1F-4891-9183-5065833A50E0}"/>
+    <hyperlink ref="L20" r:id="rId11" xr:uid="{01765EFA-C62C-4B91-A88F-D5874520DE32}"/>
+    <hyperlink ref="L22" r:id="rId12" xr:uid="{079666C0-A4CD-4E76-8A19-014C03E31646}"/>
+    <hyperlink ref="L23" r:id="rId13" xr:uid="{C95657F0-E9BA-495D-B9B8-74DBD1BD2E75}"/>
+    <hyperlink ref="L24" r:id="rId14" xr:uid="{EB0A38F8-0E8C-4BA4-9215-8CA91405624B}"/>
+    <hyperlink ref="L25" r:id="rId15" xr:uid="{5384F591-C02D-46A6-954E-B4CE2280FEAA}"/>
+    <hyperlink ref="L26" r:id="rId16" xr:uid="{D492D089-928B-40D3-BE74-C50A31A7067E}"/>
+    <hyperlink ref="L27" r:id="rId17" xr:uid="{A107BB3A-DA8C-44DB-8451-1865404A85EA}"/>
+    <hyperlink ref="L28" r:id="rId18" xr:uid="{90B56A92-25E4-40DB-942F-4A8F1E7F86AD}"/>
+    <hyperlink ref="L29" r:id="rId19" xr:uid="{06E57685-4A92-47E7-AC5F-5F28C7DD74E7}"/>
+    <hyperlink ref="L30" r:id="rId20" xr:uid="{E43A8064-E3DC-4619-9E76-324BF4A6D56C}"/>
+    <hyperlink ref="L31" r:id="rId21" xr:uid="{B1404575-24BB-4813-A1C3-2CC6D5C3FE73}"/>
+    <hyperlink ref="L32" r:id="rId22" xr:uid="{D6F3AAAC-B6A6-4CC6-B4F7-824D9B1EC4BF}"/>
+    <hyperlink ref="L33" r:id="rId23" xr:uid="{BE5E205E-7E20-4415-AFCE-59664F123447}"/>
+    <hyperlink ref="S14" r:id="rId24" xr:uid="{C5A9DC7D-DA14-4651-A46A-DD450C679617}"/>
+    <hyperlink ref="S15" r:id="rId25" xr:uid="{3EBACCBA-4F72-43AB-AED9-A02753D9D3B7}"/>
+    <hyperlink ref="S17" r:id="rId26" xr:uid="{D28B2EA8-441E-4E21-8E3A-652E8E0BF9A9}"/>
+    <hyperlink ref="S18" r:id="rId27" xr:uid="{2AE1CC9D-AFBA-47FC-AF09-8CA6CD295A73}"/>
+    <hyperlink ref="S16" r:id="rId28" xr:uid="{2561DDBA-E562-4D14-9763-BDD719C54522}"/>
+    <hyperlink ref="S22" r:id="rId29" xr:uid="{55FDE6BE-2B9D-4441-AEFE-2778C59BA426}"/>
+    <hyperlink ref="S20" r:id="rId30" xr:uid="{026ED3B6-E7CF-4871-BC83-12BEE0C44E8A}"/>
+    <hyperlink ref="S19" r:id="rId31" xr:uid="{CD30C8F4-BD61-44C5-9F0D-00EE87665DA7}"/>
+    <hyperlink ref="S21" r:id="rId32" xr:uid="{D40524B1-EFD4-43E6-A770-6E06288C6B3F}"/>
+    <hyperlink ref="S23" r:id="rId33" xr:uid="{7586DA2F-168B-4401-8C8A-58787FD1AC87}"/>
+    <hyperlink ref="S24" r:id="rId34" xr:uid="{773F378D-45F2-4907-9241-1BC7E19C73AA}"/>
+    <hyperlink ref="S25" r:id="rId35" xr:uid="{50CF87C5-3E1E-4077-B270-4FA39F4754F5}"/>
+    <hyperlink ref="S26" r:id="rId36" xr:uid="{2BE70702-2F5B-46C6-B4EF-E4413E3AF5AB}"/>
+    <hyperlink ref="S27" r:id="rId37" xr:uid="{90463A52-7CE8-4EA7-9E4A-38EEA25060A7}"/>
+    <hyperlink ref="S28" r:id="rId38" xr:uid="{1B8D9E72-408F-4F68-AF2B-1AE148157921}"/>
+    <hyperlink ref="S29" r:id="rId39" xr:uid="{CDFC554A-6BF8-4A07-BBC3-395902AE4F29}"/>
+    <hyperlink ref="S30" r:id="rId40" xr:uid="{C1E427A4-B7ED-4CCE-9418-0A22C89157C0}"/>
+    <hyperlink ref="S31" r:id="rId41" xr:uid="{0E63F9C9-C60B-4EF2-9D65-980DA3EE1D32}"/>
+    <hyperlink ref="S32" r:id="rId42" xr:uid="{8BDE0F65-41CC-4AEC-8AF1-E4456F88267A}"/>
+    <hyperlink ref="S33" r:id="rId43" xr:uid="{4EEAE9C7-EAA0-4675-8521-F90423BB9B25}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
 
@@ -5352,30 +6324,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D3FDD47-2C56-4972-B83A-8FECD57E4475}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="172.7109375" customWidth="1"/>
+    <col min="2" max="2" width="172.5703125" customWidth="1"/>
     <col min="3" max="3" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" s="1" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -5391,15 +6363,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE67F289-8E83-412D-9594-E09762F1E311}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
       <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1" ht="18.75">
       <c r="A1" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>